<commit_message>
fix(api): align data with current optimization logic
</commit_message>
<xml_diff>
--- a/backend/data/z_score_table.xlsx
+++ b/backend/data/z_score_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekgibbs/Library/Mobile Documents/com~apple~CloudDocs/School/CourseCast/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\projects\CourseCast\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DB08964-647E-AE46-90CD-642CEB952235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8F0660-20AC-412C-B16C-3989CCEAF594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27940" yWindow="-1020" windowWidth="26840" windowHeight="15440" xr2:uid="{F82743B9-7144-6B40-A1D1-4FE87530D320}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F82743B9-7144-6B40-A1D1-4FE87530D320}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -408,18 +408,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5931DDF3-A916-EC42-BD1D-26C0594481E2}">
-  <dimension ref="A1:CV236"/>
+  <dimension ref="A1:CV237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0">
-      <selection activeCell="CJ9" sqref="CJ9"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A238" sqref="A238"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="100" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -721,7 +721,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>-1.7358360083697169</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>0.61133944353523939</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.40185874909228925</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>-2.6294868830986844E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>-0.70348829502598675</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0.35667298422984034</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>-3.3954245724357082E-2</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>1.9329021514536193</v>
       </c>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.15667227707768724</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>-0.55108216880599215</v>
       </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>-0.79081841358509419</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>1.0732543237868688</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1.8406766293060357</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>1.0278744427742952</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>-0.28659811169106925</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>0.93966881278086534</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.47551713973176851</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>-0.73247538190720274</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2.1251955751613094</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>0.8913716074649124</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2.4161905141221528E-3</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>-0.4419152437619599</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.56708259521602222</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0.11273546178064314</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>-0.59985584149348026</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>-0.7441121474793746</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9.1036501883172402E-2</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>-0.38376100045058231</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1.2003603909251455</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>-0.97618655839603818</v>
       </c>
     </row>
-    <row r="17" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1.4119809070024028</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>-0.79123944408100377</v>
       </c>
     </row>
-    <row r="18" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>-0.89894489794551424</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>1.1229989861925427</v>
       </c>
     </row>
-    <row r="19" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0.83405786576796903</v>
       </c>
@@ -6157,7 +6157,7 @@
         <v>-0.66534594253304469</v>
       </c>
     </row>
-    <row r="20" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0.31650204603442117</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>-1.4432656062397604</v>
       </c>
     </row>
-    <row r="21" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.61977067660489493</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>0.86751632464981498</v>
       </c>
     </row>
-    <row r="22" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>-1.6834120340214458</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>2.4947381016197374</v>
       </c>
     </row>
-    <row r="23" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.35100575312220578</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>-1.313062613364389</v>
       </c>
     </row>
-    <row r="24" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>0.85900925004757744</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>-0.54641510218367273</v>
       </c>
     </row>
-    <row r="25" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>0.47412445387750013</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>1.4290701280288305</v>
       </c>
     </row>
-    <row r="26" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>-0.11040230592424596</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>-1.189971211582926</v>
       </c>
     </row>
-    <row r="27" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>-1.2379772571711267</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>-1.203471849663351</v>
       </c>
     </row>
-    <row r="28" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>-0.31299732878998004</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>-0.20517233217212394</v>
       </c>
     </row>
-    <row r="29" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>-0.86631333972024327</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v>-1.5792716141228813</v>
       </c>
     </row>
-    <row r="30" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1.0968273875530723</v>
       </c>
@@ -9479,7 +9479,7 @@
         <v>0.89696333263050021</v>
       </c>
     </row>
-    <row r="31" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>-1.1836543813326947</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>-0.68924503417268146</v>
       </c>
     </row>
-    <row r="32" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>0.67270150101396076</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>0.9335232037308544</v>
       </c>
     </row>
-    <row r="33" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>-0.61357964536931464</v>
       </c>
@@ -10385,7 +10385,7 @@
         <v>-0.96623592898536526</v>
       </c>
     </row>
-    <row r="34" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>-0.92554911440721033</v>
       </c>
@@ -10687,7 +10687,7 @@
         <v>0.71196747764711765</v>
       </c>
     </row>
-    <row r="35" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>-0.37966114090493508</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>1.4054934014328344</v>
       </c>
     </row>
-    <row r="36" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4.8855523528076273E-3</v>
       </c>
@@ -11291,7 +11291,7 @@
         <v>-0.11672626195105172</v>
       </c>
     </row>
-    <row r="37" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>-0.38865303800334194</v>
       </c>
@@ -11593,7 +11593,7 @@
         <v>0.98189954303604343</v>
       </c>
     </row>
-    <row r="38" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>6.9324679647670112E-2</v>
       </c>
@@ -11895,7 +11895,7 @@
         <v>-2.4703531200763844E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>1.2115005864682189</v>
       </c>
@@ -12197,7 +12197,7 @@
         <v>0.87323299842168234</v>
       </c>
     </row>
-    <row r="40" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>9.4608684233780271E-2</v>
       </c>
@@ -12499,7 +12499,7 @@
         <v>-1.0279033380601039</v>
       </c>
     </row>
-    <row r="41" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>0.61520220826489203</v>
       </c>
@@ -12801,7 +12801,7 @@
         <v>0.66807708371306407</v>
       </c>
     </row>
-    <row r="42" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>0.91098909679222495</v>
       </c>
@@ -13103,7 +13103,7 @@
         <v>-0.80598965082653407</v>
       </c>
     </row>
-    <row r="43" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>-1.1273830319754581</v>
       </c>
@@ -13405,7 +13405,7 @@
         <v>-0.91986588362634536</v>
       </c>
     </row>
-    <row r="44" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>5.6713964995722309E-2</v>
       </c>
@@ -13707,7 +13707,7 @@
         <v>-0.89300812202940427</v>
       </c>
     </row>
-    <row r="45" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>-0.56608325839491047</v>
       </c>
@@ -14009,7 +14009,7 @@
         <v>-0.58823572329408547</v>
       </c>
     </row>
-    <row r="46" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>-0.11161530567916496</v>
       </c>
@@ -14311,7 +14311,7 @@
         <v>0.61326640894258333</v>
       </c>
     </row>
-    <row r="47" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>-0.10551478627488031</v>
       </c>
@@ -14613,7 +14613,7 @@
         <v>0.84889869894074632</v>
       </c>
     </row>
-    <row r="48" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>-0.70443414429133855</v>
       </c>
@@ -14915,7 +14915,7 @@
         <v>0.97729338196831816</v>
       </c>
     </row>
-    <row r="49" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>1.0225027565301741</v>
       </c>
@@ -15217,7 +15217,7 @@
         <v>1.8488093305146318</v>
       </c>
     </row>
-    <row r="50" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>-0.63935968790628983</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>-0.2562171173209728</v>
       </c>
     </row>
-    <row r="51" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>-1.238963182861387</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>-0.59499015496299523</v>
       </c>
     </row>
-    <row r="52" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>0.87997100697445896</v>
       </c>
@@ -16123,7 +16123,7 @@
         <v>-1.9699993423524966</v>
       </c>
     </row>
-    <row r="53" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>-0.99449505225406942</v>
       </c>
@@ -16425,7 +16425,7 @@
         <v>1.6552676576395022</v>
       </c>
     </row>
-    <row r="54" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>0.13049281638498048</v>
       </c>
@@ -16727,7 +16727,7 @@
         <v>0.23110581885029594</v>
       </c>
     </row>
-    <row r="55" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>-8.9160456114387235E-2</v>
       </c>
@@ -17029,7 +17029,7 @@
         <v>-0.64472162074783612</v>
       </c>
     </row>
-    <row r="56" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>-0.82502603357373239</v>
       </c>
@@ -17331,7 +17331,7 @@
         <v>0.64231283904628489</v>
       </c>
     </row>
-    <row r="57" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>-0.15567003473718227</v>
       </c>
@@ -17633,7 +17633,7 @@
         <v>0.64818964859256545</v>
       </c>
     </row>
-    <row r="58" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>1.0384207950706033</v>
       </c>
@@ -17935,7 +17935,7 @@
         <v>-0.37782887431406131</v>
       </c>
     </row>
-    <row r="59" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>-0.59032784443128683</v>
       </c>
@@ -18237,7 +18237,7 @@
         <v>-7.7063556528293243E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>-0.19881860382916089</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>0.59847778904135829</v>
       </c>
     </row>
-    <row r="61" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>1.2851892903674103</v>
       </c>
@@ -18841,7 +18841,7 @@
         <v>1.8459056233957161</v>
       </c>
     </row>
-    <row r="62" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>-0.2280947151139382</v>
       </c>
@@ -19143,7 +19143,7 @@
         <v>-4.1848621401053838E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>1.3981828300766868</v>
       </c>
@@ -19445,7 +19445,7 @@
         <v>1.9298968176150856E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>-0.2854252920535334</v>
       </c>
@@ -19747,7 +19747,7 @@
         <v>-0.41952271463908319</v>
       </c>
     </row>
-    <row r="65" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>-1.5461373810841004</v>
       </c>
@@ -20049,7 +20049,7 @@
         <v>-0.48489809993505262</v>
       </c>
     </row>
-    <row r="66" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>0.59449818863263504</v>
       </c>
@@ -20351,7 +20351,7 @@
         <v>-0.28654143859451531</v>
       </c>
     </row>
-    <row r="67" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>-0.43429844200136614</v>
       </c>
@@ -20653,7 +20653,7 @@
         <v>0.97373140065418773</v>
       </c>
     </row>
-    <row r="68" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1.2781960308473013</v>
       </c>
@@ -20955,7 +20955,7 @@
         <v>-0.83621242261191309</v>
       </c>
     </row>
-    <row r="69" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>6.156673985912902E-2</v>
       </c>
@@ -21257,7 +21257,7 @@
         <v>-0.89419704025497393</v>
       </c>
     </row>
-    <row r="70" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>-0.82060472603894741</v>
       </c>
@@ -21559,7 +21559,7 @@
         <v>0.77038836765962182</v>
       </c>
     </row>
-    <row r="71" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>1.4464353193684079</v>
       </c>
@@ -21861,7 +21861,7 @@
         <v>1.7946657112387088</v>
       </c>
     </row>
-    <row r="72" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>-0.79943954752795687</v>
       </c>
@@ -22163,7 +22163,7 @@
         <v>-0.61542003825102409</v>
       </c>
     </row>
-    <row r="73" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>-0.57833099995803028</v>
       </c>
@@ -22465,7 +22465,7 @@
         <v>0.95451715728754016</v>
       </c>
     </row>
-    <row r="74" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>0.33774221811448901</v>
       </c>
@@ -22767,7 +22767,7 @@
         <v>-0.33899469136757049</v>
       </c>
     </row>
-    <row r="75" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>-2.1796210628919681</v>
       </c>
@@ -23069,7 +23069,7 @@
         <v>0.27348339609263589</v>
       </c>
     </row>
-    <row r="76" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>0.38344850772085537</v>
       </c>
@@ -23371,7 +23371,7 @@
         <v>-0.23902900262540994</v>
       </c>
     </row>
-    <row r="77" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>0.27540857614902425</v>
       </c>
@@ -23673,7 +23673,7 @@
         <v>0.74952591857267115</v>
       </c>
     </row>
-    <row r="78" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>1.6925370706130618</v>
       </c>
@@ -23975,7 +23975,7 @@
         <v>-2.7035876300450323</v>
       </c>
     </row>
-    <row r="79" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>-0.55590332913890594</v>
       </c>
@@ -24277,7 +24277,7 @@
         <v>0.63002224654038164</v>
       </c>
     </row>
-    <row r="80" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>-0.91675371966724273</v>
       </c>
@@ -24579,7 +24579,7 @@
         <v>-0.33360224672231431</v>
       </c>
     </row>
-    <row r="81" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>-0.39430125259093063</v>
       </c>
@@ -24881,7 +24881,7 @@
         <v>-0.21042619050008501</v>
       </c>
     </row>
-    <row r="82" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>0.84382604772921044</v>
       </c>
@@ -25183,7 +25183,7 @@
         <v>-0.5866979129151898</v>
       </c>
     </row>
-    <row r="83" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>-0.6613619804640789</v>
       </c>
@@ -25485,7 +25485,7 @@
         <v>0.4982062014785647</v>
       </c>
     </row>
-    <row r="84" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>1.5682341454122524</v>
       </c>
@@ -25787,7 +25787,7 @@
         <v>0.46709380194978839</v>
       </c>
     </row>
-    <row r="85" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>1.019487126450497</v>
       </c>
@@ -26089,7 +26089,7 @@
         <v>-0.24496442413826466</v>
       </c>
     </row>
-    <row r="86" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>2.155096482686774</v>
       </c>
@@ -26391,7 +26391,7 @@
         <v>-0.97658691203660486</v>
       </c>
     </row>
-    <row r="87" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>-1.703703024365476</v>
       </c>
@@ -26693,7 +26693,7 @@
         <v>0.16919587087077703</v>
       </c>
     </row>
-    <row r="88" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>2.2193381467103159</v>
       </c>
@@ -26995,7 +26995,7 @@
         <v>1.1536634901737608</v>
       </c>
     </row>
-    <row r="89" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>-0.76970895813580353</v>
       </c>
@@ -27297,7 +27297,7 @@
         <v>2.2155838083294803</v>
       </c>
     </row>
-    <row r="90" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>-0.93779173673342731</v>
       </c>
@@ -27599,7 +27599,7 @@
         <v>-0.71696147885127748</v>
       </c>
     </row>
-    <row r="91" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>-1.4166162606241073</v>
       </c>
@@ -27901,7 +27901,7 @@
         <v>-0.98886750886957808</v>
       </c>
     </row>
-    <row r="92" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>1.0676420536061306</v>
       </c>
@@ -28203,7 +28203,7 @@
         <v>-0.55112072995930694</v>
       </c>
     </row>
-    <row r="93" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>1.4459407921033156</v>
       </c>
@@ -28505,7 +28505,7 @@
         <v>0.84040042309628793</v>
       </c>
     </row>
-    <row r="94" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>-0.55163364592871544</v>
       </c>
@@ -28807,7 +28807,7 @@
         <v>-2.6269296481713367</v>
       </c>
     </row>
-    <row r="95" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>-0.6924161942442818</v>
       </c>
@@ -29109,7 +29109,7 @@
         <v>-0.95221903377819994</v>
       </c>
     </row>
-    <row r="96" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>-0.73312778366212317</v>
       </c>
@@ -29411,7 +29411,7 @@
         <v>1.0980403296927581</v>
       </c>
     </row>
-    <row r="97" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>-1.5544337515475837</v>
       </c>
@@ -29713,7 +29713,7 @@
         <v>1.1609984081293911</v>
       </c>
     </row>
-    <row r="98" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>8.0839257436705642E-2</v>
       </c>
@@ -30015,7 +30015,7 @@
         <v>0.26902383817766939</v>
       </c>
     </row>
-    <row r="99" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>-1.9052714148537329</v>
       </c>
@@ -30317,7 +30317,7 @@
         <v>-0.21213834002661819</v>
       </c>
     </row>
-    <row r="100" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>-0.50621622484823525</v>
       </c>
@@ -30619,7 +30619,7 @@
         <v>0.68792041296996098</v>
       </c>
     </row>
-    <row r="101" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>-0.56415781294184475</v>
       </c>
@@ -30921,7 +30921,7 @@
         <v>0.18685800937227937</v>
       </c>
     </row>
-    <row r="102" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>-4.5879770447400194E-2</v>
       </c>
@@ -31223,7 +31223,7 @@
         <v>-0.6586650140303737</v>
       </c>
     </row>
-    <row r="103" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>-0.32309390606693705</v>
       </c>
@@ -31525,7 +31525,7 @@
         <v>1.2938276835187839</v>
       </c>
     </row>
-    <row r="104" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>-0.87206126305558629</v>
       </c>
@@ -31827,7 +31827,7 @@
         <v>-0.81314719483095488</v>
       </c>
     </row>
-    <row r="105" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>1.7815372957965714</v>
       </c>
@@ -32129,7 +32129,7 @@
         <v>1.115540236431257</v>
       </c>
     </row>
-    <row r="106" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>-0.68749533552240727</v>
       </c>
@@ -32431,7 +32431,7 @@
         <v>1.3659944051138424</v>
       </c>
     </row>
-    <row r="107" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>-1.327477955356398</v>
       </c>
@@ -32733,7 +32733,7 @@
         <v>0.84235222483784811</v>
       </c>
     </row>
-    <row r="108" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>-0.50321398852654542</v>
       </c>
@@ -33035,7 +33035,7 @@
         <v>-1.5709051563254524</v>
       </c>
     </row>
-    <row r="109" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>0.67171774930346928</v>
       </c>
@@ -33337,7 +33337,7 @@
         <v>-0.86322559189679948</v>
       </c>
     </row>
-    <row r="110" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>0.69077490133527808</v>
       </c>
@@ -33639,7 +33639,7 @@
         <v>1.2221602246335503</v>
       </c>
     </row>
-    <row r="111" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>1.2270855114027688</v>
       </c>
@@ -33941,7 +33941,7 @@
         <v>0.24484945780878128</v>
       </c>
     </row>
-    <row r="112" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>-0.57202346605618359</v>
       </c>
@@ -34243,7 +34243,7 @@
         <v>1.9402863114819071</v>
       </c>
     </row>
-    <row r="113" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>6.080832910154757E-2</v>
       </c>
@@ -34545,7 +34545,7 @@
         <v>-0.16018818251453484</v>
       </c>
     </row>
-    <row r="114" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>-1.3872679231968774</v>
       </c>
@@ -34847,7 +34847,7 @@
         <v>-0.44762986793864801</v>
       </c>
     </row>
-    <row r="115" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>-0.29373573659678048</v>
       </c>
@@ -35149,7 +35149,7 @@
         <v>-0.43794269096062344</v>
       </c>
     </row>
-    <row r="116" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>-3.8595158815533825E-2</v>
       </c>
@@ -35451,7 +35451,7 @@
         <v>0.28947242360401371</v>
       </c>
     </row>
-    <row r="117" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>-0.9132192990748389</v>
       </c>
@@ -35753,7 +35753,7 @@
         <v>0.88629240433274181</v>
       </c>
     </row>
-    <row r="118" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>0.69630637884531632</v>
       </c>
@@ -36055,7 +36055,7 @@
         <v>-1.001247350321423</v>
       </c>
     </row>
-    <row r="119" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>1.1140866282692539</v>
       </c>
@@ -36357,7 +36357,7 @@
         <v>-0.32127575576153128</v>
       </c>
     </row>
-    <row r="120" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>0.55799127669030513</v>
       </c>
@@ -36659,7 +36659,7 @@
         <v>-0.47959093764479904</v>
       </c>
     </row>
-    <row r="121" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>-1.4724124743710184E-3</v>
       </c>
@@ -36961,7 +36961,7 @@
         <v>1.0161924731252019</v>
       </c>
     </row>
-    <row r="122" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>9.6633704993696487E-2</v>
       </c>
@@ -37263,7 +37263,7 @@
         <v>-1.6903605339406687</v>
       </c>
     </row>
-    <row r="123" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>-1.0111685097737799</v>
       </c>
@@ -37565,7 +37565,7 @@
         <v>8.452378995814655E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>0.33717305880190507</v>
       </c>
@@ -37867,7 +37867,7 @@
         <v>-0.2913249481334369</v>
       </c>
     </row>
-    <row r="125" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>1.659640538219076</v>
       </c>
@@ -38169,7 +38169,7 @@
         <v>-0.30860878515309859</v>
       </c>
     </row>
-    <row r="126" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>-0.64766785919162395</v>
       </c>
@@ -38471,7 +38471,7 @@
         <v>-1.6510406206539647</v>
       </c>
     </row>
-    <row r="127" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>0.17498518765246276</v>
       </c>
@@ -38773,7 +38773,7 @@
         <v>0.1099885830085113</v>
       </c>
     </row>
-    <row r="128" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>1.0141106454613751</v>
       </c>
@@ -39075,7 +39075,7 @@
         <v>0.46427654758033793</v>
       </c>
     </row>
-    <row r="129" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>-1.0772804952022608</v>
       </c>
@@ -39377,7 +39377,7 @@
         <v>0.38008277536459772</v>
       </c>
     </row>
-    <row r="130" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>-0.67639523018321879</v>
       </c>
@@ -39679,7 +39679,7 @@
         <v>0.47401697054407538</v>
       </c>
     </row>
-    <row r="131" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>-0.78552301979406736</v>
       </c>
@@ -39981,7 +39981,7 @@
         <v>-0.58952988976886822</v>
       </c>
     </row>
-    <row r="132" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>-1.1055460190904887</v>
       </c>
@@ -40283,7 +40283,7 @@
         <v>-0.14573306597408703</v>
       </c>
     </row>
-    <row r="133" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>2.2932389065870602</v>
       </c>
@@ -40585,7 +40585,7 @@
         <v>-1.3458669574536797</v>
       </c>
     </row>
-    <row r="134" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>-0.89690525586503012</v>
       </c>
@@ -40887,7 +40887,7 @@
         <v>0.98869787945061804</v>
       </c>
     </row>
-    <row r="135" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>0.54733778337582073</v>
       </c>
@@ -41189,7 +41189,7 @@
         <v>7.3815233609244205E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>0.3156352331606041</v>
       </c>
@@ -41491,7 +41491,7 @@
         <v>5.5497899144240186E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>-5.5698195157883823E-2</v>
       </c>
@@ -41793,7 +41793,7 @@
         <v>1.0961376285435003</v>
       </c>
     </row>
-    <row r="138" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>0.85660233915725581</v>
       </c>
@@ -42095,7 +42095,7 @@
         <v>8.6125801350368208E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>-0.72683317439038286</v>
       </c>
@@ -42397,7 +42397,7 @@
         <v>-6.454969424295566E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>-3.7629064702589782E-2</v>
       </c>
@@ -42699,7 +42699,7 @@
         <v>-0.62218833621796277</v>
       </c>
     </row>
-    <row r="141" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>-0.3789708976958594</v>
       </c>
@@ -43001,7 +43001,7 @@
         <v>-0.95989273989023149</v>
       </c>
     </row>
-    <row r="142" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>0.89544602313664001</v>
       </c>
@@ -43303,7 +43303,7 @@
         <v>-1.3681327636183731</v>
       </c>
     </row>
-    <row r="143" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>1.0108977226010543</v>
       </c>
@@ -43605,7 +43605,7 @@
         <v>-2.6262666768051113</v>
       </c>
     </row>
-    <row r="144" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>-0.71842049740850256</v>
       </c>
@@ -43907,7 +43907,7 @@
         <v>-0.3712641805025742</v>
       </c>
     </row>
-    <row r="145" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>5.7664787320472616E-2</v>
       </c>
@@ -44209,7 +44209,7 @@
         <v>-0.88037169292190243</v>
       </c>
     </row>
-    <row r="146" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>-0.34821533009890338</v>
       </c>
@@ -44511,7 +44511,7 @@
         <v>-0.59096182966285737</v>
       </c>
     </row>
-    <row r="147" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>-1.0137557164323692</v>
       </c>
@@ -44813,7 +44813,7 @@
         <v>-0.38944038240351303</v>
       </c>
     </row>
-    <row r="148" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>0.56385400152329967</v>
       </c>
@@ -45115,7 +45115,7 @@
         <v>0.95295659495583851</v>
       </c>
     </row>
-    <row r="149" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>1.2169233953673417</v>
       </c>
@@ -45417,7 +45417,7 @@
         <v>0.5090271263404611</v>
       </c>
     </row>
-    <row r="150" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>0.11800419538221465</v>
       </c>
@@ -45719,7 +45719,7 @@
         <v>2.5878689075198209</v>
       </c>
     </row>
-    <row r="151" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>-0.3625255984213584</v>
       </c>
@@ -46021,7 +46021,7 @@
         <v>1.018703405627164</v>
       </c>
     </row>
-    <row r="152" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>0.78302988914757243</v>
       </c>
@@ -46323,7 +46323,7 @@
         <v>0.55007733132957359</v>
       </c>
     </row>
-    <row r="153" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>0.42675638501791774</v>
       </c>
@@ -46625,7 +46625,7 @@
         <v>1.6972548975174417</v>
       </c>
     </row>
-    <row r="154" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>0.18836101809561698</v>
       </c>
@@ -46927,7 +46927,7 @@
         <v>0.84691653207263096</v>
       </c>
     </row>
-    <row r="155" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>-0.30383598801407169</v>
       </c>
@@ -47229,7 +47229,7 @@
         <v>-0.52966072535335285</v>
       </c>
     </row>
-    <row r="156" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>-8.0941640150991881E-2</v>
       </c>
@@ -47531,7 +47531,7 @@
         <v>1.6627074797294881</v>
       </c>
     </row>
-    <row r="157" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>-0.67094333621527524</v>
       </c>
@@ -47833,7 +47833,7 @@
         <v>-0.22645072749291753</v>
       </c>
     </row>
-    <row r="158" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>0.14942646727434292</v>
       </c>
@@ -48135,7 +48135,7 @@
         <v>1.5047833858481479</v>
       </c>
     </row>
-    <row r="159" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>-0.51204123395023282</v>
       </c>
@@ -48437,7 +48437,7 @@
         <v>0.50691644480640263</v>
       </c>
     </row>
-    <row r="160" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>-3.4711992269511729E-2</v>
       </c>
@@ -48739,7 +48739,7 @@
         <v>-0.42336016908485102</v>
       </c>
     </row>
-    <row r="161" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>0.29574575846544093</v>
       </c>
@@ -49041,7 +49041,7 @@
         <v>-0.50915830193486178</v>
       </c>
     </row>
-    <row r="162" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>-4.5284881416298592E-2</v>
       </c>
@@ -49343,7 +49343,7 @@
         <v>-0.6176221974734375</v>
       </c>
     </row>
-    <row r="163" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>-1.03763685294631</v>
       </c>
@@ -49645,7 +49645,7 @@
         <v>-1.0533494409021274E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>-0.98495019440046583</v>
       </c>
@@ -49947,7 +49947,7 @@
         <v>0.96768672464069294</v>
       </c>
     </row>
-    <row r="165" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>0.71501490340810803</v>
       </c>
@@ -50249,7 +50249,7 @@
         <v>0.92570837240350801</v>
       </c>
     </row>
-    <row r="166" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>0.65886103130885887</v>
       </c>
@@ -50551,7 +50551,7 @@
         <v>0.87008550330145384</v>
       </c>
     </row>
-    <row r="167" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>0.16112029129400854</v>
       </c>
@@ -50853,7 +50853,7 @@
         <v>0.10892021967885686</v>
       </c>
     </row>
-    <row r="168" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>-1.9259053298906292</v>
       </c>
@@ -51155,7 +51155,7 @@
         <v>0.89883451967182015</v>
       </c>
     </row>
-    <row r="169" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>0.34024672295446817</v>
       </c>
@@ -51457,7 +51457,7 @@
         <v>-1.4542917240534923</v>
       </c>
     </row>
-    <row r="170" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>4.3761610131274392E-3</v>
       </c>
@@ -51759,7 +51759,7 @@
         <v>1.6362019442512485</v>
       </c>
     </row>
-    <row r="171" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>0.12662722443081115</v>
       </c>
@@ -52061,7 +52061,7 @@
         <v>-0.51616506615521807</v>
       </c>
     </row>
-    <row r="172" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>0.96463265096303319</v>
       </c>
@@ -52363,7 +52363,7 @@
         <v>1.7049295540373601</v>
       </c>
     </row>
-    <row r="173" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>2.7028904772465938</v>
       </c>
@@ -52665,7 +52665,7 @@
         <v>0.24230419425767061</v>
       </c>
     </row>
-    <row r="174" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>0.66834734493617087</v>
       </c>
@@ -52967,7 +52967,7 @@
         <v>2.1030281099427732</v>
       </c>
     </row>
-    <row r="175" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>0.17959434776340069</v>
       </c>
@@ -53269,7 +53269,7 @@
         <v>0.94247932723681183</v>
       </c>
     </row>
-    <row r="176" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>1.161888897107914</v>
       </c>
@@ -53571,7 +53571,7 @@
         <v>0.13739273718124004</v>
       </c>
     </row>
-    <row r="177" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>-0.60201476155301648</v>
       </c>
@@ -53873,7 +53873,7 @@
         <v>-1.0502006075443979</v>
       </c>
     </row>
-    <row r="178" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>1.0433779837452914</v>
       </c>
@@ -54175,7 +54175,7 @@
         <v>-0.31576062188908832</v>
       </c>
     </row>
-    <row r="179" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>0.46691391442586816</v>
       </c>
@@ -54477,7 +54477,7 @@
         <v>-0.1663063678881275</v>
       </c>
     </row>
-    <row r="180" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>-0.99298818560415936</v>
       </c>
@@ -54779,7 +54779,7 @@
         <v>-0.58481641025808007</v>
       </c>
     </row>
-    <row r="181" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>-0.75450384021531325</v>
       </c>
@@ -55081,7 +55081,7 @@
         <v>1.9267732970355782</v>
       </c>
     </row>
-    <row r="182" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>-1.0987079622940872</v>
       </c>
@@ -55383,7 +55383,7 @@
         <v>1.1284989893901576</v>
       </c>
     </row>
-    <row r="183" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>2.2371944778543118</v>
       </c>
@@ -55685,7 +55685,7 @@
         <v>-2.2997864810357225</v>
       </c>
     </row>
-    <row r="184" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>1.8187894619367517</v>
       </c>
@@ -55987,7 +55987,7 @@
         <v>-1.1807434466935538</v>
       </c>
     </row>
-    <row r="185" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>-0.94740736530979408</v>
       </c>
@@ -56289,7 +56289,7 @@
         <v>-1.1579721179390965</v>
       </c>
     </row>
-    <row r="186" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>-1.5253449746620023</v>
       </c>
@@ -56591,7 +56591,7 @@
         <v>0.96683323363490437</v>
       </c>
     </row>
-    <row r="187" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>1.0581179278612641E-2</v>
       </c>
@@ -56893,7 +56893,7 @@
         <v>-0.30923309528842047</v>
       </c>
     </row>
-    <row r="188" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>-2.7421463658962879</v>
       </c>
@@ -57195,7 +57195,7 @@
         <v>0.36166264143399102</v>
       </c>
     </row>
-    <row r="189" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>1.8712406234441501</v>
       </c>
@@ -57497,7 +57497,7 @@
         <v>-1.5041772219031204</v>
       </c>
     </row>
-    <row r="190" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>-0.78538421247981305</v>
       </c>
@@ -57799,7 +57799,7 @@
         <v>3.1054404624753312E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>1.3551997765065034</v>
       </c>
@@ -58101,7 +58101,7 @@
         <v>-0.49722495810544814</v>
       </c>
     </row>
-    <row r="192" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>-1.3140352379473217</v>
       </c>
@@ -58403,7 +58403,7 @@
         <v>-5.4336685621575898E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>-0.97535314795701811</v>
       </c>
@@ -58705,7 +58705,7 @@
         <v>-0.48735621114701416</v>
       </c>
     </row>
-    <row r="194" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>1.5890999914457915</v>
       </c>
@@ -59007,7 +59007,7 @@
         <v>0.51229750407788188</v>
       </c>
     </row>
-    <row r="195" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>-2.5422642187545872</v>
       </c>
@@ -59309,7 +59309,7 @@
         <v>0.58586123386117439</v>
       </c>
     </row>
-    <row r="196" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>1.4101910175777601</v>
       </c>
@@ -59611,7 +59611,7 @@
         <v>1.753716964018406</v>
       </c>
     </row>
-    <row r="197" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>-2.8764948594373098E-2</v>
       </c>
@@ -59913,7 +59913,7 @@
         <v>-0.73507844974795433</v>
       </c>
     </row>
-    <row r="198" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>-4.3354129716564063E-2</v>
       </c>
@@ -60215,7 +60215,7 @@
         <v>3.0125945894461013</v>
       </c>
     </row>
-    <row r="199" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>0.67317480345416481</v>
       </c>
@@ -60517,7 +60517,7 @@
         <v>-0.92935400711957949</v>
       </c>
     </row>
-    <row r="200" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>0.40757461512858073</v>
       </c>
@@ -60819,7 +60819,7 @@
         <v>-0.34107109630514587</v>
       </c>
     </row>
-    <row r="201" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>0.84994021834831768</v>
       </c>
@@ -61121,7 +61121,7 @@
         <v>-1.2340939132260016</v>
       </c>
     </row>
-    <row r="202" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>-1.4451349444097827</v>
       </c>
@@ -61423,7 +61423,7 @@
         <v>3.2677179477425926E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>-0.23317589842894784</v>
       </c>
@@ -61725,7 +61725,7 @@
         <v>-0.11029574419736761</v>
       </c>
     </row>
-    <row r="204" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>0.98417529025505845</v>
       </c>
@@ -62027,7 +62027,7 @@
         <v>-1.7831900316599492</v>
       </c>
     </row>
-    <row r="205" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>2.0463208836452687</v>
       </c>
@@ -62329,7 +62329,7 @@
         <v>0.86096392551342427</v>
       </c>
     </row>
-    <row r="206" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>0.65690752931645136</v>
       </c>
@@ -62631,7 +62631,7 @@
         <v>-0.68276097025267612</v>
       </c>
     </row>
-    <row r="207" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>-0.46650036086791408</v>
       </c>
@@ -62933,7 +62933,7 @@
         <v>-2.0605559996126321</v>
       </c>
     </row>
-    <row r="208" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>-0.51552686436476491</v>
       </c>
@@ -63235,7 +63235,7 @@
         <v>-2.8138598299378126</v>
       </c>
     </row>
-    <row r="209" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>-0.48003151772401081</v>
       </c>
@@ -63537,7 +63537,7 @@
         <v>-0.36643324708347774</v>
       </c>
     </row>
-    <row r="210" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>0.97981996982945185</v>
       </c>
@@ -63839,7 +63839,7 @@
         <v>-4.7536469311632197E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>0.9311330394213484</v>
       </c>
@@ -64141,7 +64141,7 @@
         <v>3.4534008530629434E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>1.0881209454172782</v>
       </c>
@@ -64443,7 +64443,7 @@
         <v>1.3590376517472174</v>
       </c>
     </row>
-    <row r="213" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>-1.2379378879344702</v>
       </c>
@@ -64745,7 +64745,7 @@
         <v>0.89837016654742463</v>
       </c>
     </row>
-    <row r="214" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>0.83379417628610275</v>
       </c>
@@ -65047,7 +65047,7 @@
         <v>-0.16251245440699699</v>
       </c>
     </row>
-    <row r="215" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>1.320081797123922</v>
       </c>
@@ -65349,7 +65349,7 @@
         <v>2.2244405859604997</v>
       </c>
     </row>
-    <row r="216" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>1.0483316056384342</v>
       </c>
@@ -65651,7 +65651,7 @@
         <v>-0.81513724285994249</v>
       </c>
     </row>
-    <row r="217" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>1.5488810179310466</v>
       </c>
@@ -65953,7 +65953,7 @@
         <v>-0.50775607609520557</v>
       </c>
     </row>
-    <row r="218" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>-0.8618186462378159</v>
       </c>
@@ -66255,7 +66255,7 @@
         <v>-0.70934146903094197</v>
       </c>
     </row>
-    <row r="219" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>-1.137895882295596</v>
       </c>
@@ -66557,7 +66557,7 @@
         <v>0.24711948536645084</v>
       </c>
     </row>
-    <row r="220" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>-1.4971405877573258</v>
       </c>
@@ -66859,7 +66859,7 @@
         <v>0.73785302125675023</v>
       </c>
     </row>
-    <row r="221" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>-0.88399031851601573</v>
       </c>
@@ -67161,7 +67161,7 @@
         <v>4.139163995868253E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>1.2154537045539233</v>
       </c>
@@ -67463,7 +67463,7 @@
         <v>-1.120921751044994</v>
       </c>
     </row>
-    <row r="223" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>0.63367753509754021</v>
       </c>
@@ -67765,7 +67765,7 @@
         <v>0.256204034833029</v>
       </c>
     </row>
-    <row r="224" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>-0.47526215786683618</v>
       </c>
@@ -68067,7 +68067,7 @@
         <v>-0.91935379159405839</v>
       </c>
     </row>
-    <row r="225" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>0.30805017953233954</v>
       </c>
@@ -68369,7 +68369,7 @@
         <v>0.37306835256482335</v>
       </c>
     </row>
-    <row r="226" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>0.56115914034768122</v>
       </c>
@@ -68671,7 +68671,7 @@
         <v>0.39785385948830854</v>
       </c>
     </row>
-    <row r="227" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>1.3217464940467376</v>
       </c>
@@ -68973,7 +68973,7 @@
         <v>-0.91103594434521029</v>
       </c>
     </row>
-    <row r="228" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>-0.60137738813899944</v>
       </c>
@@ -69275,7 +69275,7 @@
         <v>-1.1696330139352857</v>
       </c>
     </row>
-    <row r="229" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>1.3459795613634444</v>
       </c>
@@ -69577,7 +69577,7 @@
         <v>6.6365405747042139E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>-0.77775305210068835</v>
       </c>
@@ -69879,7 +69879,7 @@
         <v>-1.4802006082410031</v>
       </c>
     </row>
-    <row r="231" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>-0.39582764989069685</v>
       </c>
@@ -70181,7 +70181,7 @@
         <v>1.4589277021781795</v>
       </c>
     </row>
-    <row r="232" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>-2.1686565294007769</v>
       </c>
@@ -70483,7 +70483,7 @@
         <v>4.5821868470636143E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>0.60823805654269247</v>
       </c>
@@ -70785,7 +70785,7 @@
         <v>-2.1718852972815941</v>
       </c>
     </row>
-    <row r="234" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>-1.1773335871092396</v>
       </c>
@@ -71087,7 +71087,7 @@
         <v>-1.9710474690925222</v>
       </c>
     </row>
-    <row r="235" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>0.43633256570674406</v>
       </c>
@@ -71389,7 +71389,7 @@
         <v>-0.78709000918656602</v>
       </c>
     </row>
-    <row r="236" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>-1.2798413620700078</v>
       </c>
@@ -71688,6 +71688,308 @@
         <v>0.1115986062126125</v>
       </c>
       <c r="CV236" s="1">
+        <v>0.39868822683833022</v>
+      </c>
+    </row>
+    <row r="237" spans="1:100" x14ac:dyDescent="0.3">
+      <c r="A237" s="1">
+        <v>-1.2798413620700078</v>
+      </c>
+      <c r="B237" s="1">
+        <v>0.34844969282391092</v>
+      </c>
+      <c r="C237" s="1">
+        <v>1.3626987796606227</v>
+      </c>
+      <c r="D237" s="1">
+        <v>-0.18860742790245355</v>
+      </c>
+      <c r="E237" s="1">
+        <v>1.3329194277105181</v>
+      </c>
+      <c r="F237" s="1">
+        <v>-7.3720501471748245E-2</v>
+      </c>
+      <c r="G237" s="1">
+        <v>0.67951961941394401</v>
+      </c>
+      <c r="H237" s="1">
+        <v>0.1310285429012007</v>
+      </c>
+      <c r="I237" s="1">
+        <v>1.808707102800081</v>
+      </c>
+      <c r="J237" s="1">
+        <v>-6.1347748785882443E-2</v>
+      </c>
+      <c r="K237" s="1">
+        <v>1.9846308691318699</v>
+      </c>
+      <c r="L237" s="1">
+        <v>-1.6885583247951494</v>
+      </c>
+      <c r="M237" s="1">
+        <v>0.36870276480735137</v>
+      </c>
+      <c r="N237" s="1">
+        <v>-0.84615346875314335</v>
+      </c>
+      <c r="O237" s="1">
+        <v>4.9803585497692281E-2</v>
+      </c>
+      <c r="P237" s="1">
+        <v>-0.36320815697276115</v>
+      </c>
+      <c r="Q237" s="1">
+        <v>-1.76236411950966</v>
+      </c>
+      <c r="R237" s="1">
+        <v>-0.68706737306172438</v>
+      </c>
+      <c r="S237" s="1">
+        <v>0.7759611634109429</v>
+      </c>
+      <c r="T237" s="1">
+        <v>-1.5073076220811559</v>
+      </c>
+      <c r="U237" s="1">
+        <v>-0.6788718441504088</v>
+      </c>
+      <c r="V237" s="1">
+        <v>0.45181131682101106</v>
+      </c>
+      <c r="W237" s="1">
+        <v>-0.21494667140692564</v>
+      </c>
+      <c r="X237" s="1">
+        <v>0.28861353025641018</v>
+      </c>
+      <c r="Y237" s="1">
+        <v>-0.71782834608830692</v>
+      </c>
+      <c r="Z237" s="1">
+        <v>-0.11516406623434303</v>
+      </c>
+      <c r="AA237" s="1">
+        <v>-1.1642943867420619</v>
+      </c>
+      <c r="AB237" s="1">
+        <v>-0.40924127544567601</v>
+      </c>
+      <c r="AC237" s="1">
+        <v>-0.27803960136135913</v>
+      </c>
+      <c r="AD237" s="1">
+        <v>1.3836201658999354</v>
+      </c>
+      <c r="AE237" s="1">
+        <v>-0.12998275822974095</v>
+      </c>
+      <c r="AF237" s="1">
+        <v>-5.5294783393060397E-2</v>
+      </c>
+      <c r="AG237" s="1">
+        <v>-1.2776260568041879</v>
+      </c>
+      <c r="AH237" s="1">
+        <v>-2.1025763648364872</v>
+      </c>
+      <c r="AI237" s="1">
+        <v>-0.27849770997158657</v>
+      </c>
+      <c r="AJ237" s="1">
+        <v>0.93571801387399411</v>
+      </c>
+      <c r="AK237" s="1">
+        <v>-0.26772367363823324</v>
+      </c>
+      <c r="AL237" s="1">
+        <v>0.48029228140765901</v>
+      </c>
+      <c r="AM237" s="1">
+        <v>0.66368626296809607</v>
+      </c>
+      <c r="AN237" s="1">
+        <v>0.26939661760045552</v>
+      </c>
+      <c r="AO237" s="1">
+        <v>-0.21090309421112988</v>
+      </c>
+      <c r="AP237" s="1">
+        <v>-1.3098882533544098</v>
+      </c>
+      <c r="AQ237" s="1">
+        <v>-0.74136912838626468</v>
+      </c>
+      <c r="AR237" s="1">
+        <v>0.13359427240696622</v>
+      </c>
+      <c r="AS237" s="1">
+        <v>1.8149077087069891</v>
+      </c>
+      <c r="AT237" s="1">
+        <v>0.47678615859679535</v>
+      </c>
+      <c r="AU237" s="1">
+        <v>1.3454465714533692</v>
+      </c>
+      <c r="AV237" s="1">
+        <v>-2.3967969286110304</v>
+      </c>
+      <c r="AW237" s="1">
+        <v>-2.6683192399571491</v>
+      </c>
+      <c r="AX237" s="1">
+        <v>-1.4059091209878538</v>
+      </c>
+      <c r="AY237" s="1">
+        <v>0.74018213591854276</v>
+      </c>
+      <c r="AZ237" s="1">
+        <v>-0.14714714462004028</v>
+      </c>
+      <c r="BA237" s="1">
+        <v>0.85041726433068909</v>
+      </c>
+      <c r="BB237" s="1">
+        <v>1.1408931927460919</v>
+      </c>
+      <c r="BC237" s="1">
+        <v>-6.2597793682347205E-2</v>
+      </c>
+      <c r="BD237" s="1">
+        <v>0.4573339647325288</v>
+      </c>
+      <c r="BE237" s="1">
+        <v>-0.88356030488772541</v>
+      </c>
+      <c r="BF237" s="1">
+        <v>1.2546810010817846</v>
+      </c>
+      <c r="BG237" s="1">
+        <v>0.96634271600461907</v>
+      </c>
+      <c r="BH237" s="1">
+        <v>0.41298320543068079</v>
+      </c>
+      <c r="BI237" s="1">
+        <v>-1.5748066364001145</v>
+      </c>
+      <c r="BJ237" s="1">
+        <v>1.4175708171631745</v>
+      </c>
+      <c r="BK237" s="1">
+        <v>-0.96853033653049714</v>
+      </c>
+      <c r="BL237" s="1">
+        <v>-1.2493931475546372</v>
+      </c>
+      <c r="BM237" s="1">
+        <v>1.9948045527429623</v>
+      </c>
+      <c r="BN237" s="1">
+        <v>0.20878184064266195</v>
+      </c>
+      <c r="BO237" s="1">
+        <v>-0.60818656644117264</v>
+      </c>
+      <c r="BP237" s="1">
+        <v>3.1497371236227178</v>
+      </c>
+      <c r="BQ237" s="1">
+        <v>1.1546401594512334</v>
+      </c>
+      <c r="BR237" s="1">
+        <v>9.5130577787860285E-2</v>
+      </c>
+      <c r="BS237" s="1">
+        <v>-0.81015841937396815</v>
+      </c>
+      <c r="BT237" s="1">
+        <v>-1.2289716864537019</v>
+      </c>
+      <c r="BU237" s="1">
+        <v>-1.0586350975398253</v>
+      </c>
+      <c r="BV237" s="1">
+        <v>4.4487631876200542E-2</v>
+      </c>
+      <c r="BW237" s="1">
+        <v>0.41622946613215478</v>
+      </c>
+      <c r="BX237" s="1">
+        <v>-0.78347143099595906</v>
+      </c>
+      <c r="BY237" s="1">
+        <v>0.89101909114482436</v>
+      </c>
+      <c r="BZ237" s="1">
+        <v>0.46286989662133415</v>
+      </c>
+      <c r="CA237" s="1">
+        <v>-1.5268263942443219</v>
+      </c>
+      <c r="CB237" s="1">
+        <v>9.5589780424393311E-2</v>
+      </c>
+      <c r="CC237" s="1">
+        <v>-0.26944897161521736</v>
+      </c>
+      <c r="CD237" s="1">
+        <v>1.5283766058219326</v>
+      </c>
+      <c r="CE237" s="1">
+        <v>-1.7824853428073169</v>
+      </c>
+      <c r="CF237" s="1">
+        <v>0.20146597827815901</v>
+      </c>
+      <c r="CG237" s="1">
+        <v>-1.7664624197461655E-2</v>
+      </c>
+      <c r="CH237" s="1">
+        <v>-0.1735062123345649</v>
+      </c>
+      <c r="CI237" s="1">
+        <v>-0.74790084815755731</v>
+      </c>
+      <c r="CJ237" s="1">
+        <v>0.51374348392040681</v>
+      </c>
+      <c r="CK237" s="1">
+        <v>0.25292483332202592</v>
+      </c>
+      <c r="CL237" s="1">
+        <v>0.86691252594673796</v>
+      </c>
+      <c r="CM237" s="1">
+        <v>-0.74254274911984819</v>
+      </c>
+      <c r="CN237" s="1">
+        <v>-1.4576265911845672</v>
+      </c>
+      <c r="CO237" s="1">
+        <v>-1.080103612938206</v>
+      </c>
+      <c r="CP237" s="1">
+        <v>0.4603280969633492</v>
+      </c>
+      <c r="CQ237" s="1">
+        <v>-1.2132437114968784</v>
+      </c>
+      <c r="CR237" s="1">
+        <v>-1.060929127275777</v>
+      </c>
+      <c r="CS237" s="1">
+        <v>-0.18784224756684673</v>
+      </c>
+      <c r="CT237" s="1">
+        <v>-0.14179919915429173</v>
+      </c>
+      <c r="CU237" s="1">
+        <v>0.1115986062126125</v>
+      </c>
+      <c r="CV237" s="1">
         <v>0.39868822683833022</v>
       </c>
     </row>

</xml_diff>